<commit_message>
Added code for Most Likely Tagger
</commit_message>
<xml_diff>
--- a/HW02/Workbook2.xlsx
+++ b/HW02/Workbook2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="13960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>2 776</t>
   </si>
@@ -43,18 +43,53 @@
   <si>
     <t>1 1399</t>
   </si>
+  <si>
+    <t>brown</t>
+  </si>
+  <si>
+    <t>treebank</t>
+  </si>
+  <si>
+    <t>all words</t>
+  </si>
+  <si>
+    <t>words with out punct's</t>
+  </si>
+  <si>
+    <t>oovs</t>
+  </si>
+  <si>
+    <t>top10 Highest Entropy words</t>
+  </si>
+  <si>
+    <t>MLE</t>
+  </si>
+  <si>
+    <t>Laplace</t>
+  </si>
+  <si>
+    <t>Witten Bell</t>
+  </si>
+  <si>
+    <t>Simple Good Turing</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
     </font>
   </fonts>
   <fills count="2">
@@ -77,8 +112,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -301,11 +337,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2146043472"/>
-        <c:axId val="-2146040512"/>
+        <c:axId val="-2088893152"/>
+        <c:axId val="-2095871776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2146043472"/>
+        <c:axId val="-2088893152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -362,12 +398,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2146040512"/>
+        <c:crossAx val="-2095871776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2146040512"/>
+        <c:axId val="-2095871776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -424,7 +460,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2146043472"/>
+        <c:crossAx val="-2088893152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -518,7 +554,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -639,11 +674,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2134515440"/>
-        <c:axId val="-2134508272"/>
+        <c:axId val="-2070634720"/>
+        <c:axId val="-2070417664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2134515440"/>
+        <c:axId val="-2070634720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -700,12 +735,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2134508272"/>
+        <c:crossAx val="-2070417664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2134508272"/>
+        <c:axId val="-2070417664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -762,7 +797,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2134515440"/>
+        <c:crossAx val="-2070634720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -774,6 +809,885 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Train Data Subset(%)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Vs Accuracy(%)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="dbl" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="34925" cap="flat" cmpd="dbl" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                    <a:alpha val="70000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$4:$P$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$4:$Q$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77.73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80.26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>83.97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>86.96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87.31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>88.03</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>88.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>89.34</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>89.82</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2070104288"/>
+        <c:axId val="-2070101040"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2070104288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2070101040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2070101040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2070104288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$W$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>all words</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$X$3:$AA$3</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MLE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Laplace</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Witten Bell</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Simple Good Turing</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$X$4:$AA$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>29.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>89.82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89.74</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$W$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>oovs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$X$3:$AA$3</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MLE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Laplace</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Witten Bell</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Simple Good Turing</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$X$5:$AA$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>24.260815437286</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37.5816993464052</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50.2645502645502</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50.2956738250855</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$W$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>words with out punct's</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$X$3:$AA$3</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MLE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Laplace</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Witten Bell</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Simple Good Turing</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$X$6:$AA$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>31.0768062760976</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78.1222320637732</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88.36644312286469</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>88.371504491965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$W$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>top10 Highest Entropy words</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$X$3:$AA$3</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MLE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Laplace</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Witten Bell</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Simple Good Turing</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$X$7:$AA$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>19.626168224299</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55.1401869158878</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.4859813084112</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62.6168224299065</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2071453008"/>
+        <c:axId val="-2095955392"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2071453008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2095955392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2095955392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2071453008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -891,6 +1805,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1904,6 +2898,1025 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="243">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="flat" cmpd="dbl" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="flat" cmpd="dbl" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+            <a:alpha val="70000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" kern="1200" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1980,6 +3993,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2251,15 +4324,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:AA30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="23" max="23" width="27.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -2273,7 +4349,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -2287,7 +4363,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -2300,8 +4376,20 @@
       <c r="E3">
         <v>187</v>
       </c>
+      <c r="X3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -2314,8 +4402,29 @@
       <c r="E4">
         <v>35</v>
       </c>
+      <c r="P4">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>68</v>
+      </c>
+      <c r="W4" t="s">
+        <v>8</v>
+      </c>
+      <c r="X4" s="1">
+        <v>29.32</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>80.97</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>89.82</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>89.74</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -2337,8 +4446,29 @@
       <c r="N5">
         <v>776</v>
       </c>
+      <c r="P5">
+        <v>20</v>
+      </c>
+      <c r="Q5">
+        <v>77.73</v>
+      </c>
+      <c r="W5" t="s">
+        <v>10</v>
+      </c>
+      <c r="X5" s="1">
+        <v>24.260815437285999</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>37.581699346405202</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>50.264550264550202</v>
+      </c>
+      <c r="AA5">
+        <v>50.295673825085501</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6</v>
       </c>
@@ -2360,8 +4490,29 @@
       <c r="N6">
         <v>187</v>
       </c>
+      <c r="P6">
+        <v>30</v>
+      </c>
+      <c r="Q6">
+        <v>80.260000000000005</v>
+      </c>
+      <c r="W6" t="s">
+        <v>9</v>
+      </c>
+      <c r="X6" s="1">
+        <v>31.076806276097599</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>78.122232063773197</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>88.366443122864695</v>
+      </c>
+      <c r="AA6">
+        <v>88.371504491964998</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
@@ -2383,8 +4534,29 @@
       <c r="N7">
         <v>35</v>
       </c>
+      <c r="P7">
+        <v>40</v>
+      </c>
+      <c r="Q7">
+        <v>83.97</v>
+      </c>
+      <c r="W7" t="s">
+        <v>11</v>
+      </c>
+      <c r="X7" s="1">
+        <v>19.626168224299001</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>55.140186915887803</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>64.485981308411198</v>
+      </c>
+      <c r="AA7">
+        <v>62.616822429906499</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2406,8 +4578,14 @@
       <c r="N8">
         <v>6</v>
       </c>
+      <c r="P8">
+        <v>50</v>
+      </c>
+      <c r="Q8">
+        <v>86.96</v>
+      </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
@@ -2429,8 +4607,14 @@
       <c r="N9">
         <v>1</v>
       </c>
+      <c r="P9">
+        <v>60</v>
+      </c>
+      <c r="Q9">
+        <v>87.31</v>
+      </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
@@ -2446,8 +4630,14 @@
       <c r="I10" t="s">
         <v>4</v>
       </c>
+      <c r="P10">
+        <v>70</v>
+      </c>
+      <c r="Q10">
+        <v>88.03</v>
+      </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>11</v>
       </c>
@@ -2460,8 +4650,14 @@
       <c r="E11">
         <v>0</v>
       </c>
+      <c r="P11">
+        <v>80</v>
+      </c>
+      <c r="Q11">
+        <v>88.4</v>
+      </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>13</v>
       </c>
@@ -2474,8 +4670,14 @@
       <c r="E12">
         <v>0</v>
       </c>
+      <c r="P12">
+        <v>90</v>
+      </c>
+      <c r="Q12">
+        <v>89.34</v>
+      </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>15</v>
       </c>
@@ -2487,6 +4689,22 @@
       </c>
       <c r="E13">
         <v>0</v>
+      </c>
+      <c r="P13">
+        <v>100</v>
+      </c>
+      <c r="Q13">
+        <v>89.82</v>
+      </c>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="K27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>